<commit_message>
added better envolpe stuff, why!
</commit_message>
<xml_diff>
--- a/Progress-Check/Timeline.xlsx
+++ b/Progress-Check/Timeline.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B786293D-6CAB-47F0-A8C3-18A3DA089893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F89659-AE72-481A-AABF-593BA0B0BA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Phase 1 Title</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>Filter Component</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>No In Scope</t>
+  </si>
+  <si>
+    <t>Not in Scope</t>
   </si>
 </sst>
 </file>
@@ -910,6 +919,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -922,13 +938,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1499,7 +1508,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1550,341 +1559,341 @@
       <c r="B3" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="90">
+      <c r="D3" s="88"/>
+      <c r="E3" s="93">
         <f ca="1">TODAY()</f>
-        <v>44286</v>
-      </c>
-      <c r="F3" s="90"/>
+        <v>44311</v>
+      </c>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="90">
         <f ca="1">I5</f>
-        <v>44284</v>
-      </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+        <v>44312</v>
+      </c>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f ca="1">P5</f>
-        <v>44291</v>
-      </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+        <v>44319</v>
+      </c>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f ca="1">W5</f>
-        <v>44298</v>
-      </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+        <v>44326</v>
+      </c>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f ca="1">AD5</f>
-        <v>44305</v>
-      </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+        <v>44333</v>
+      </c>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f ca="1">AK5</f>
-        <v>44312</v>
-      </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+        <v>44340</v>
+      </c>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f ca="1">AR5</f>
-        <v>44319</v>
-      </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+        <v>44347</v>
+      </c>
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f ca="1">AY5</f>
-        <v>44326</v>
-      </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="87">
+        <v>44354</v>
+      </c>
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f ca="1">BF5</f>
-        <v>44333</v>
-      </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
+        <v>44361</v>
+      </c>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44284</v>
+        <v>44312</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44285</v>
+        <v>44313</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44286</v>
+        <v>44314</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44287</v>
+        <v>44315</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44288</v>
+        <v>44316</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44289</v>
+        <v>44317</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44290</v>
+        <v>44318</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44291</v>
+        <v>44319</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44292</v>
+        <v>44320</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44293</v>
+        <v>44321</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44294</v>
+        <v>44322</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44295</v>
+        <v>44323</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44296</v>
+        <v>44324</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44297</v>
+        <v>44325</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>44298</v>
+        <v>44326</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>44299</v>
+        <v>44327</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44300</v>
+        <v>44328</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44301</v>
+        <v>44329</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44302</v>
+        <v>44330</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44303</v>
+        <v>44331</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44304</v>
+        <v>44332</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>44305</v>
+        <v>44333</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>44306</v>
+        <v>44334</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44307</v>
+        <v>44335</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44308</v>
+        <v>44336</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44309</v>
+        <v>44337</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44310</v>
+        <v>44338</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44311</v>
+        <v>44339</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>44312</v>
+        <v>44340</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>44313</v>
+        <v>44341</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44314</v>
+        <v>44342</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44315</v>
+        <v>44343</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44316</v>
+        <v>44344</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44317</v>
+        <v>44345</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44318</v>
+        <v>44346</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>44319</v>
+        <v>44347</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>44320</v>
+        <v>44348</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44321</v>
+        <v>44349</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44322</v>
+        <v>44350</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44323</v>
+        <v>44351</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44324</v>
+        <v>44352</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44325</v>
+        <v>44353</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>44326</v>
+        <v>44354</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>44327</v>
+        <v>44355</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>44328</v>
+        <v>44356</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44329</v>
+        <v>44357</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44330</v>
+        <v>44358</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44331</v>
+        <v>44359</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>44332</v>
+        <v>44360</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>44333</v>
+        <v>44361</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>44334</v>
+        <v>44362</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>44335</v>
+        <v>44363</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44336</v>
+        <v>44364</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44337</v>
+        <v>44365</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44338</v>
+        <v>44366</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>44339</v>
+        <v>44367</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2282,18 +2291,16 @@
       <c r="B9" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="72"/>
+      <c r="C9" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="D9" s="22"/>
-      <c r="E9" s="66">
-        <v>44277</v>
-      </c>
-      <c r="F9" s="66">
-        <v>44291</v>
-      </c>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="17">
+      <c r="H9" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v/>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2359,18 +2366,16 @@
       <c r="B10" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="72"/>
+      <c r="C10" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="66">
-        <v>44277</v>
-      </c>
-      <c r="F10" s="66">
-        <v>44284</v>
-      </c>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="17">
+      <c r="H10" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="44"/>
@@ -2434,18 +2439,16 @@
       <c r="B11" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="66">
-        <v>44291</v>
-      </c>
-      <c r="F11" s="66">
-        <v>44298</v>
-      </c>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="17">
+      <c r="H11" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I11" s="44"/>
       <c r="J11" s="44"/>
@@ -2509,18 +2512,16 @@
       <c r="B12" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="66">
-        <v>44291</v>
-      </c>
-      <c r="F12" s="66">
-        <v>44298</v>
-      </c>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="17">
+      <c r="H12" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -2584,18 +2585,16 @@
       <c r="B13" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="72"/>
+      <c r="C13" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="66">
-        <v>44298</v>
-      </c>
-      <c r="F13" s="66">
-        <v>44305</v>
-      </c>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="17">
+      <c r="H13" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
@@ -2732,18 +2731,16 @@
       <c r="B15" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="74"/>
+      <c r="C15" s="74" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="67">
-        <v>44298</v>
-      </c>
-      <c r="F15" s="67">
-        <v>44305</v>
-      </c>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="17">
+      <c r="H15" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
@@ -2810,15 +2807,15 @@
       <c r="C16" s="74"/>
       <c r="D16" s="27"/>
       <c r="E16" s="67">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="F16" s="67">
-        <v>44312</v>
+        <v>44326</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
@@ -2882,19 +2879,16 @@
       <c r="B17" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="74" t="s">
+        <v>60</v>
+      </c>
       <c r="D17" s="27"/>
-      <c r="E17" s="67">
-        <f>F16</f>
-        <v>44312</v>
-      </c>
-      <c r="F17" s="67">
-        <v>44319</v>
-      </c>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="17">
+      <c r="H17" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -4111,11 +4105,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4123,6 +4112,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>